<commit_message>
Remove natural escapement data (to be drawn from a different source file)
</commit_message>
<xml_diff>
--- a/1. data files/FSAR_4-panel_data.xlsx
+++ b/1. data files/FSAR_4-panel_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\WCVI-CN-ResDoc\FSAR 4-panel plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\WCVI-CN-ResDoc\1. data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4454888-0130-4134-9DD4-D28DBC5CFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496CA64A-5584-4375-A643-60100C0B813D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,31 +35,10 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={153CCB2C-F42F-4A7D-B305-15DCCCF87D47}</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{153CCB2C-F42F-4A7D-B305-15DCCCF87D47}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    From the 17 natural indicator rivers</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>nat_escapement</t>
   </si>
   <si>
     <t>ocean_catch</t>
@@ -121,9 +100,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Nicholas Brown" id="{986F2ACE-37D6-4917-9A7A-A6A346D17295}" userId="S::Nicholas.Brown@dfo-mpo.gc.ca::632ebe77-6995-4958-bf06-abfc772d892a" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,25 +364,17 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2024-04-16T23:29:23.33" personId="{986F2ACE-37D6-4917-9A7A-A6A346D17295}" id="{153CCB2C-F42F-4A7D-B305-15DCCCF87D47}">
-    <text>From the 17 natural indicator rivers</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,624 +384,485 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1979</v>
       </c>
-      <c r="B2">
-        <v>4342.2344444444443</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>0.62798842499999996</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1980</v>
       </c>
-      <c r="B3">
-        <v>9873.3104952350241</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>0.76827633399999995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1981</v>
       </c>
-      <c r="B4">
-        <v>7757.7920634920638</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>0.73571767899999996</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1982</v>
       </c>
-      <c r="B5">
-        <v>10201.78173185951</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>0.65244785999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1983</v>
       </c>
-      <c r="B6">
-        <v>5661.329557713053</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>0.75765146500000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1984</v>
       </c>
-      <c r="B7">
-        <v>7454.889411764706</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>0.75568564999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1985</v>
       </c>
       <c r="B8">
-        <v>6242.570323464136</v>
+        <v>178052.85652432509</v>
       </c>
       <c r="C8">
-        <v>178052.85652432509</v>
-      </c>
-      <c r="D8">
         <v>0.67942554899999996</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1986</v>
       </c>
       <c r="B9">
-        <v>6343.3141752345346</v>
+        <v>61106.378035804024</v>
       </c>
       <c r="C9">
-        <v>61106.378035804024</v>
-      </c>
-      <c r="D9">
         <v>0.64320170099999996</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1987</v>
       </c>
       <c r="B10">
-        <v>4381.2786665148406</v>
+        <v>45762.702178710068</v>
       </c>
       <c r="C10">
-        <v>45762.702178710068</v>
-      </c>
-      <c r="D10">
         <v>0.26142261100000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1988</v>
       </c>
       <c r="B11">
-        <v>8304.1557164567494</v>
+        <v>91527.209684412024</v>
       </c>
       <c r="C11">
-        <v>91527.209684412024</v>
-      </c>
-      <c r="D11">
         <v>0.34751590100000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1989</v>
       </c>
       <c r="B12">
-        <v>9538.8294966236954</v>
+        <v>101042.00068755817</v>
       </c>
       <c r="C12">
-        <v>101042.00068755817</v>
-      </c>
-      <c r="D12">
         <v>0.28997511999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1990</v>
       </c>
       <c r="B13">
-        <v>8246.9237875997551</v>
+        <v>196190.27181940814</v>
       </c>
       <c r="C13">
-        <v>196190.27181940814</v>
-      </c>
-      <c r="D13">
         <v>0.34718398900000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1991</v>
       </c>
       <c r="B14">
-        <v>8648.7993462867216</v>
+        <v>272793.05672136648</v>
       </c>
       <c r="C14">
-        <v>272793.05672136648</v>
-      </c>
-      <c r="D14">
         <v>0.49107056799999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1992</v>
       </c>
       <c r="B15">
-        <v>10161.952704403269</v>
+        <v>509000.80816585355</v>
       </c>
       <c r="C15">
-        <v>509000.80816585355</v>
-      </c>
-      <c r="D15">
         <v>0.63934258300000002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1993</v>
       </c>
       <c r="B16">
-        <v>11291.19643953346</v>
+        <v>277035.93881388317</v>
       </c>
       <c r="C16">
-        <v>277035.93881388317</v>
-      </c>
-      <c r="D16">
         <v>0.59468891599999996</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1994</v>
       </c>
       <c r="B17">
-        <v>11938.563842848371</v>
+        <v>177866.08154183425</v>
       </c>
       <c r="C17">
-        <v>177866.08154183425</v>
-      </c>
-      <c r="D17">
         <v>0.64058026199999996</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1995</v>
       </c>
       <c r="B18">
-        <v>6353</v>
+        <v>42515.378397203545</v>
       </c>
       <c r="C18">
-        <v>42515.378397203545</v>
-      </c>
-      <c r="D18">
         <v>0.58439851300000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1996</v>
       </c>
       <c r="B19">
-        <v>10609</v>
+        <v>29222.436046453673</v>
       </c>
       <c r="C19">
-        <v>29222.436046453673</v>
-      </c>
-      <c r="D19">
         <v>0.21791869699999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1997</v>
       </c>
       <c r="B20">
-        <v>14176</v>
+        <v>83599.592797319347</v>
       </c>
       <c r="C20">
-        <v>83599.592797319347</v>
-      </c>
-      <c r="D20">
         <v>0.247923591</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1998</v>
       </c>
       <c r="B21">
-        <v>29840</v>
+        <v>124815.11032298941</v>
       </c>
       <c r="C21">
-        <v>124815.11032298941</v>
-      </c>
-      <c r="D21">
         <v>0.37600623100000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1999</v>
       </c>
       <c r="B22">
-        <v>20847</v>
+        <v>65090.186561109469</v>
       </c>
       <c r="C22">
-        <v>65090.186561109469</v>
-      </c>
-      <c r="D22">
         <v>0.563086753</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2000</v>
       </c>
       <c r="B23">
-        <v>8110</v>
+        <v>9283.2749094746905</v>
       </c>
       <c r="C23">
-        <v>9283.2749094746905</v>
-      </c>
-      <c r="D23">
         <v>0.38669400599999998</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2001</v>
       </c>
       <c r="B24">
-        <v>8565.2738095238092</v>
+        <v>11749.098533839046</v>
       </c>
       <c r="C24">
-        <v>11749.098533839046</v>
-      </c>
-      <c r="D24">
         <v>7.0410851999999996E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2002</v>
       </c>
       <c r="B25">
-        <v>22123</v>
+        <v>61427.136870085698</v>
       </c>
       <c r="C25">
-        <v>61427.136870085698</v>
-      </c>
-      <c r="D25">
         <v>0.21321663399999999</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2003</v>
       </c>
       <c r="B26">
-        <v>26789</v>
+        <v>81911.385482238082</v>
       </c>
       <c r="C26">
-        <v>81911.385482238082</v>
-      </c>
-      <c r="D26">
         <v>0.21493885400000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2004</v>
       </c>
       <c r="B27">
-        <v>23272</v>
+        <v>143580.23948566156</v>
       </c>
       <c r="C27">
-        <v>143580.23948566156</v>
-      </c>
-      <c r="D27">
         <v>0.34575744400000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2005</v>
       </c>
       <c r="B28">
-        <v>8608.9995395948426</v>
+        <v>103258.77184158686</v>
       </c>
       <c r="C28">
-        <v>103258.77184158686</v>
-      </c>
-      <c r="D28">
         <v>0.40466605100000003</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2006</v>
       </c>
       <c r="B29">
-        <v>13582.08695652174</v>
+        <v>90916.999103899143</v>
       </c>
       <c r="C29">
-        <v>90916.999103899143</v>
-      </c>
-      <c r="D29">
         <v>0.34295819999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2007</v>
       </c>
       <c r="B30">
-        <v>7977.826086956522</v>
+        <v>92774.171285073113</v>
       </c>
       <c r="C30">
-        <v>92774.171285073113</v>
-      </c>
-      <c r="D30">
         <v>0.44592135100000002</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2008</v>
       </c>
       <c r="B31">
-        <v>6683</v>
+        <v>31922.274973775915</v>
       </c>
       <c r="C31">
-        <v>31922.274973775915</v>
-      </c>
-      <c r="D31">
         <v>0.35146423500000001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2009</v>
       </c>
       <c r="B32">
-        <v>13856.95652173913</v>
+        <v>72462.402256321846</v>
       </c>
       <c r="C32">
-        <v>72462.402256321846</v>
-      </c>
-      <c r="D32">
         <v>0.48343202800000001</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2010</v>
       </c>
       <c r="B33">
-        <v>10932</v>
+        <v>40984.53283981343</v>
       </c>
       <c r="C33">
-        <v>40984.53283981343</v>
-      </c>
-      <c r="D33">
         <v>0.30033380500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2011</v>
       </c>
       <c r="B34">
-        <v>11295</v>
+        <v>92469.933435721759</v>
       </c>
       <c r="C34">
-        <v>92469.933435721759</v>
-      </c>
-      <c r="D34">
         <v>0.34518059099999998</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2012</v>
       </c>
       <c r="B35">
-        <v>8652.9524375743167</v>
+        <v>41653.449926746223</v>
       </c>
       <c r="C35">
-        <v>41653.449926746223</v>
-      </c>
-      <c r="D35">
         <v>0.43071284199999998</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2013</v>
       </c>
       <c r="B36">
-        <v>17803</v>
+        <v>87812.369036630058</v>
       </c>
       <c r="C36">
-        <v>87812.369036630058</v>
-      </c>
-      <c r="D36">
         <v>0.32861700599999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2014</v>
       </c>
       <c r="B37">
-        <v>13288</v>
+        <v>69557.409547255767</v>
       </c>
       <c r="C37">
-        <v>69557.409547255767</v>
-      </c>
-      <c r="D37">
         <v>0.44020615299999999</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2015</v>
       </c>
       <c r="B38">
-        <v>23619.470868014268</v>
+        <v>87019.245961369161</v>
       </c>
       <c r="C38">
-        <v>87019.245961369161</v>
-      </c>
-      <c r="D38">
         <v>0.25517959899999998</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2016</v>
       </c>
       <c r="B39">
-        <v>23162</v>
+        <v>130058.17072369857</v>
       </c>
       <c r="C39">
-        <v>130058.17072369857</v>
-      </c>
-      <c r="D39">
         <v>0.38341636899999998</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2017</v>
       </c>
       <c r="B40">
-        <v>18250</v>
+        <v>113806.20961372726</v>
       </c>
       <c r="C40">
-        <v>113806.20961372726</v>
-      </c>
-      <c r="D40">
         <v>0.43962685099999999</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2018</v>
       </c>
       <c r="B41">
-        <v>13737</v>
+        <v>93631.047296952456</v>
       </c>
       <c r="C41">
-        <v>93631.047296952456</v>
-      </c>
-      <c r="D41">
         <v>0.30269774599999999</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2019</v>
       </c>
       <c r="B42">
-        <v>16721.621375781691</v>
+        <v>100071.49063461184</v>
       </c>
       <c r="C42">
-        <v>100071.49063461184</v>
-      </c>
-      <c r="D42">
         <v>0.36600726700000003</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2020</v>
       </c>
       <c r="B43">
-        <v>20125</v>
+        <v>68648.098394354951</v>
       </c>
       <c r="C43">
-        <v>68648.098394354951</v>
-      </c>
-      <c r="D43">
         <v>0.28084114100000002</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2021</v>
       </c>
       <c r="B44">
-        <v>21689</v>
+        <v>90895.461868662154</v>
       </c>
       <c r="C44">
-        <v>90895.461868662154</v>
-      </c>
-      <c r="D44">
         <v>0.31995095899999998</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2022</v>
       </c>
       <c r="B45">
-        <v>18243</v>
+        <v>160604.8106129762</v>
       </c>
       <c r="C45">
-        <v>160604.8106129762</v>
-      </c>
-      <c r="D45">
         <v>0.40610734500000001</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2023</v>
       </c>
       <c r="B46">
-        <v>33612.247299602037</v>
+        <v>83986.667958935839</v>
       </c>
       <c r="C46">
-        <v>83986.667958935839</v>
-      </c>
-      <c r="D46">
         <v>0.234145889</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>